<commit_message>
Sending reports using Outlook
</commit_message>
<xml_diff>
--- a/UIStudiox/Currency-Converter_Working-Files/Currency_converter/Report.xlsx
+++ b/UIStudiox/Currency-Converter_Working-Files/Currency_converter/Report.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -319,7 +319,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Marcin Szydłowski" refreshedDate="43943.062520949075" createdVersion="1" refreshedVersion="6" recordCount="50">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Marcin Szydłowski" refreshedDate="43943.685727777774" createdVersion="1" refreshedVersion="6" recordCount="50">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F1048576" sheet="Report"/>
   </cacheSource>
@@ -347,7 +347,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Total sales USD" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1154.2729999999999" maxValue="244546.63200000001"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1141.9934999999998" maxValue="244546.63200000001"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -366,7 +366,7 @@
     <s v="EUR"/>
     <n v="6691"/>
     <x v="0"/>
-    <n v="81610.796099999992"/>
+    <n v="80862.073199999999"/>
   </r>
   <r>
     <s v="Chocolate - Pistoles, White"/>
@@ -374,7 +374,7 @@
     <s v="EUR"/>
     <n v="537"/>
     <x v="0"/>
-    <n v="10208.155200000001"/>
+    <n v="10114.502400000001"/>
   </r>
   <r>
     <s v="Lemons"/>
@@ -382,7 +382,7 @@
     <s v="EUR"/>
     <n v="3966"/>
     <x v="0"/>
-    <n v="59310.736800000006"/>
+    <n v="58766.601600000009"/>
   </r>
   <r>
     <s v="Cheese - Colby"/>
@@ -390,7 +390,7 @@
     <s v="EUR"/>
     <n v="2532"/>
     <x v="0"/>
-    <n v="18711.986400000002"/>
+    <n v="18540.316800000001"/>
   </r>
   <r>
     <s v="Pepper - Orange"/>
@@ -398,7 +398,7 @@
     <s v="NOK"/>
     <n v="5441"/>
     <x v="1"/>
-    <n v="1247.94776"/>
+    <n v="1234.6717199999998"/>
   </r>
   <r>
     <s v="Star Anise, Whole"/>
@@ -406,7 +406,7 @@
     <s v="EUR"/>
     <n v="2088"/>
     <x v="0"/>
-    <n v="28039.334400000003"/>
+    <n v="27782.092800000002"/>
   </r>
   <r>
     <s v="Puff Pastry - Slab"/>
@@ -414,7 +414,7 @@
     <s v="EUR"/>
     <n v="4438"/>
     <x v="0"/>
-    <n v="30233.875000000004"/>
+    <n v="29956.500000000004"/>
   </r>
   <r>
     <s v="Mints - Striped Red"/>
@@ -422,7 +422,7 @@
     <s v="EUR"/>
     <n v="4947"/>
     <x v="0"/>
-    <n v="45887.877300000007"/>
+    <n v="45466.887600000002"/>
   </r>
   <r>
     <s v="Sprouts - Baby Pea Tendrils"/>
@@ -430,7 +430,7 @@
     <s v="EUR"/>
     <n v="4382"/>
     <x v="0"/>
-    <n v="141237.55660000001"/>
+    <n v="139941.79920000001"/>
   </r>
   <r>
     <s v="Heavy Duty Dust Pan"/>
@@ -438,7 +438,7 @@
     <s v="NOK"/>
     <n v="5073"/>
     <x v="1"/>
-    <n v="4935.5216999999993"/>
+    <n v="4883.0161499999995"/>
   </r>
   <r>
     <s v="Sprouts Dikon"/>
@@ -446,7 +446,7 @@
     <s v="NOK"/>
     <n v="6265"/>
     <x v="1"/>
-    <n v="14481.296900000001"/>
+    <n v="14327.24055"/>
   </r>
   <r>
     <s v="Chocolate - Milk"/>
@@ -454,7 +454,7 @@
     <s v="NOK"/>
     <n v="3822"/>
     <x v="1"/>
-    <n v="2069.3836799999999"/>
+    <n v="2047.3689599999998"/>
   </r>
   <r>
     <s v="Crab Meat Claw PastGBPise"/>
@@ -462,7 +462,7 @@
     <s v="EUR"/>
     <n v="4851"/>
     <x v="0"/>
-    <n v="7085.3706000000011"/>
+    <n v="7020.3672000000006"/>
   </r>
   <r>
     <s v="Lettuce - Curly Endive"/>
@@ -470,7 +470,7 @@
     <s v="EUR"/>
     <n v="374"/>
     <x v="2"/>
-    <n v="8128.7404000000006"/>
+    <n v="8054.1648000000014"/>
   </r>
   <r>
     <s v="Myers Planters Punch"/>
@@ -478,7 +478,7 @@
     <s v="EUR"/>
     <n v="7464"/>
     <x v="0"/>
-    <n v="3498.3768000000005"/>
+    <n v="3466.2816000000003"/>
   </r>
   <r>
     <s v="Rootbeer"/>
@@ -486,7 +486,7 @@
     <s v="EUR"/>
     <n v="7161"/>
     <x v="0"/>
-    <n v="174296.59169999999"/>
+    <n v="172697.5404"/>
   </r>
   <r>
     <s v="Urban Zen Drinks"/>
@@ -494,7 +494,7 @@
     <s v="EUR"/>
     <n v="1785"/>
     <x v="0"/>
-    <n v="26168.9925"/>
+    <n v="25928.910000000003"/>
   </r>
   <r>
     <s v="Iced Tea - Lemon, 460 Ml"/>
@@ -502,7 +502,7 @@
     <s v="EUR"/>
     <n v="43"/>
     <x v="0"/>
-    <n v="1221.9009000000001"/>
+    <n v="1210.6908000000001"/>
   </r>
   <r>
     <s v="Bread - Flat Bread"/>
@@ -510,7 +510,7 @@
     <s v="EUR"/>
     <n v="2684"/>
     <x v="0"/>
-    <n v="3803.2280000000005"/>
+    <n v="3768.3360000000007"/>
   </r>
   <r>
     <s v="Petit Baguette"/>
@@ -518,7 +518,7 @@
     <s v="EUR"/>
     <n v="1965"/>
     <x v="0"/>
-    <n v="53653.342500000006"/>
+    <n v="53161.11"/>
   </r>
   <r>
     <s v="Cheese Cloth No 100"/>
@@ -526,7 +526,7 @@
     <s v="EUR"/>
     <n v="2477"/>
     <x v="2"/>
-    <n v="6263.8375999999998"/>
+    <n v="6206.3711999999996"/>
   </r>
   <r>
     <s v="Wine - Chateauneuf Du Pape"/>
@@ -542,7 +542,7 @@
     <s v="EUR"/>
     <n v="502"/>
     <x v="0"/>
-    <n v="10544.158599999999"/>
+    <n v="10447.423199999999"/>
   </r>
   <r>
     <s v="Onions - White"/>
@@ -550,7 +550,7 @@
     <s v="EUR"/>
     <n v="3636"/>
     <x v="0"/>
-    <n v="106928.21520000001"/>
+    <n v="105947.2224"/>
   </r>
   <r>
     <s v="Towel Multifold"/>
@@ -558,7 +558,7 @@
     <s v="EUR"/>
     <n v="3372"/>
     <x v="0"/>
-    <n v="52155.061200000004"/>
+    <n v="51676.574400000005"/>
   </r>
   <r>
     <s v="Marzipan 50/50"/>
@@ -574,7 +574,7 @@
     <s v="EUR"/>
     <n v="7537"/>
     <x v="0"/>
-    <n v="164306.6"/>
+    <n v="162799.20000000001"/>
   </r>
   <r>
     <s v="Yogurt - Strawberry, 175 Gr"/>
@@ -582,7 +582,7 @@
     <s v="EUR"/>
     <n v="7344"/>
     <x v="0"/>
-    <n v="116071.92000000001"/>
+    <n v="115007.04000000001"/>
   </r>
   <r>
     <s v="Pepper - Jalapeno"/>
@@ -590,7 +590,7 @@
     <s v="EUR"/>
     <n v="5267"/>
     <x v="4"/>
-    <n v="3387.2076999999999"/>
+    <n v="3356.1324"/>
   </r>
   <r>
     <s v="Vaccum Bag 10x13"/>
@@ -598,7 +598,7 @@
     <s v="EUR"/>
     <n v="5002"/>
     <x v="0"/>
-    <n v="48797.010999999999"/>
+    <n v="48349.331999999995"/>
   </r>
   <r>
     <s v="Icecream - Dstk Super Cone"/>
@@ -606,7 +606,7 @@
     <s v="EUR"/>
     <n v="1623"/>
     <x v="0"/>
-    <n v="48207.157500000001"/>
+    <n v="47764.890000000007"/>
   </r>
   <r>
     <s v="Tea - Herbal I Love Lemon"/>
@@ -614,7 +614,7 @@
     <s v="NOK"/>
     <n v="5951"/>
     <x v="1"/>
-    <n v="7579.7887000000001"/>
+    <n v="7499.15265"/>
   </r>
   <r>
     <s v="Chicken - Bones"/>
@@ -622,7 +622,7 @@
     <s v="EUR"/>
     <n v="5100"/>
     <x v="0"/>
-    <n v="52476.960000000006"/>
+    <n v="51995.520000000004"/>
   </r>
   <r>
     <s v="Tomatoes Tear Drop Yellow"/>
@@ -630,7 +630,7 @@
     <s v="EUR"/>
     <n v="5565"/>
     <x v="2"/>
-    <n v="17348.331000000002"/>
+    <n v="17189.172000000002"/>
   </r>
   <r>
     <s v="Pear - Prickly"/>
@@ -638,7 +638,7 @@
     <s v="EUR"/>
     <n v="6381"/>
     <x v="0"/>
-    <n v="12936.839400000001"/>
+    <n v="12818.1528"/>
   </r>
   <r>
     <s v="Muffin - Bran Ind Wrpd"/>
@@ -646,7 +646,7 @@
     <s v="EUR"/>
     <n v="8595"/>
     <x v="0"/>
-    <n v="139497.70950000003"/>
+    <n v="138217.91400000002"/>
   </r>
   <r>
     <s v="Sauerkraut"/>
@@ -654,7 +654,7 @@
     <s v="EUR"/>
     <n v="1480"/>
     <x v="4"/>
-    <n v="12034.472"/>
+    <n v="11924.064"/>
   </r>
   <r>
     <s v="Lemonade - Kiwi, 591 Ml"/>
@@ -662,7 +662,7 @@
     <s v="EUR"/>
     <n v="455"/>
     <x v="0"/>
-    <n v="11426.688"/>
+    <n v="11321.856"/>
   </r>
   <r>
     <s v="Lamb - Sausage Casings"/>
@@ -670,7 +670,7 @@
     <s v="EUR"/>
     <n v="3501"/>
     <x v="0"/>
-    <n v="70025.251500000013"/>
+    <n v="69382.818000000014"/>
   </r>
   <r>
     <s v="Eggplant Oriental"/>
@@ -678,7 +678,7 @@
     <s v="EUR"/>
     <n v="3793"/>
     <x v="0"/>
-    <n v="25136.9696"/>
+    <n v="24906.355200000002"/>
   </r>
   <r>
     <s v="Seedlings - Buckwheat, Organic"/>
@@ -686,7 +686,7 @@
     <s v="EUR"/>
     <n v="3633"/>
     <x v="2"/>
-    <n v="78011.409"/>
+    <n v="77295.707999999999"/>
   </r>
   <r>
     <s v="Pear - Asian"/>
@@ -694,7 +694,7 @@
     <s v="EUR"/>
     <n v="3677"/>
     <x v="0"/>
-    <n v="103524.83189999999"/>
+    <n v="102575.0628"/>
   </r>
   <r>
     <s v="Sparkling Wine - Rose, Freixenet"/>
@@ -702,7 +702,7 @@
     <s v="EUR"/>
     <n v="324"/>
     <x v="0"/>
-    <n v="7600.0032000000001"/>
+    <n v="7530.2784000000001"/>
   </r>
   <r>
     <s v="Bagels Poppyseed"/>
@@ -710,7 +710,7 @@
     <s v="NOK"/>
     <n v="3998"/>
     <x v="1"/>
-    <n v="7317.0596399999995"/>
+    <n v="7239.2185799999997"/>
   </r>
   <r>
     <s v="Pepper - Green Thai"/>
@@ -718,7 +718,7 @@
     <s v="NOK"/>
     <n v="1996"/>
     <x v="1"/>
-    <n v="3769.36616"/>
+    <n v="3729.2665200000001"/>
   </r>
   <r>
     <s v="Carbonated Water - Blackberry"/>
@@ -726,7 +726,7 @@
     <s v="NOK"/>
     <n v="5990"/>
     <x v="1"/>
-    <n v="1154.2729999999999"/>
+    <n v="1141.9934999999998"/>
   </r>
   <r>
     <s v="Shiratamako - Rice Flour"/>
@@ -734,7 +734,7 @@
     <s v="EUR"/>
     <n v="7160"/>
     <x v="0"/>
-    <n v="181296.21200000003"/>
+    <n v="179632.94400000002"/>
   </r>
   <r>
     <s v="Milk Powder"/>
@@ -742,7 +742,7 @@
     <s v="EUR"/>
     <n v="6880"/>
     <x v="0"/>
-    <n v="66592.896000000008"/>
+    <n v="65981.952000000019"/>
   </r>
   <r>
     <s v="Filling - Mince Meat"/>
@@ -764,7 +764,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Countries Sales Overview" cacheId="11" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Dane" updatedVersion="6" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" pageOverThenDown="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Countries Sales Overview" cacheId="3" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Dane" updatedVersion="6" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" pageOverThenDown="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1">
   <location ref="A1:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0" includeNewItemsInFilter="1">
@@ -1196,7 +1196,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="5">
-        <v>1902492.6054</v>
+        <v>1885038.5447999998</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1204,7 +1204,7 @@
         <v>44</v>
       </c>
       <c r="B3" s="5">
-        <v>15421.679700000001</v>
+        <v>15280.196400000001</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1212,7 +1212,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="5">
-        <v>42554.637540000003</v>
+        <v>42101.928629999995</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1220,7 +1220,7 @@
         <v>27</v>
       </c>
       <c r="B5" s="5">
-        <v>109752.318</v>
+        <v>108745.416</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1242,7 +1242,7 @@
         <v>68</v>
       </c>
       <c r="B8" s="5">
-        <v>2383646.88864</v>
+        <v>2364591.7338299998</v>
       </c>
     </row>
   </sheetData>
@@ -1305,8 +1305,8 @@
         <v>12</v>
       </c>
       <c r="F2">
-        <f>6691*11.19*1.09</f>
-        <v>81610.796099999992</v>
+        <f>6691*11.19*1.08</f>
+        <v>80862.073199999999</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -1327,8 +1327,8 @@
         <v>12</v>
       </c>
       <c r="F3">
-        <f>537*17.44*1.09</f>
-        <v>10208.155200000001</v>
+        <f>537*17.44*1.08</f>
+        <v>10114.502400000001</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -1349,8 +1349,8 @@
         <v>12</v>
       </c>
       <c r="F4">
-        <f>3966*13.72*1.09</f>
-        <v>59310.736800000006</v>
+        <f>3966*13.72*1.08</f>
+        <v>58766.601600000009</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1371,8 +1371,8 @@
         <v>12</v>
       </c>
       <c r="F5">
-        <f>2532*6.78*1.09</f>
-        <v>18711.986400000002</v>
+        <f>2532*6.78*1.08</f>
+        <v>18540.316800000001</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1393,8 +1393,8 @@
         <v>17</v>
       </c>
       <c r="F6">
-        <f>5441*2.44*0.094</f>
-        <v>1247.94776</v>
+        <f>5441*2.44*0.093</f>
+        <v>1234.6717199999998</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -1415,8 +1415,8 @@
         <v>12</v>
       </c>
       <c r="F7">
-        <f>2088*12.32*1.09</f>
-        <v>28039.334400000003</v>
+        <f>2088*12.32*1.08</f>
+        <v>27782.092800000002</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -1437,8 +1437,8 @@
         <v>12</v>
       </c>
       <c r="F8">
-        <f>4438*6.25*1.09</f>
-        <v>30233.875000000004</v>
+        <f>4438*6.25*1.08</f>
+        <v>29956.500000000004</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -1459,8 +1459,8 @@
         <v>12</v>
       </c>
       <c r="F9">
-        <f>4947*8.51*1.09</f>
-        <v>45887.877300000007</v>
+        <f>4947*8.51*1.08</f>
+        <v>45466.887600000002</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -1481,8 +1481,8 @@
         <v>12</v>
       </c>
       <c r="F10">
-        <f>4382*29.57*1.09</f>
-        <v>141237.55660000001</v>
+        <f>4382*29.57*1.08</f>
+        <v>139941.79920000001</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1503,8 +1503,8 @@
         <v>17</v>
       </c>
       <c r="F11">
-        <f>5073*10.35*0.094</f>
-        <v>4935.5216999999993</v>
+        <f>5073*10.35*0.093</f>
+        <v>4883.0161499999995</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -1525,8 +1525,8 @@
         <v>17</v>
       </c>
       <c r="F12">
-        <f>6265*24.59*0.094</f>
-        <v>14481.296900000001</v>
+        <f>6265*24.59*0.093</f>
+        <v>14327.24055</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1547,8 +1547,8 @@
         <v>17</v>
       </c>
       <c r="F13">
-        <f>3822*5.76*0.094</f>
-        <v>2069.3836799999999</v>
+        <f>3822*5.76*0.093</f>
+        <v>2047.3689599999998</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -1569,8 +1569,8 @@
         <v>12</v>
       </c>
       <c r="F14">
-        <f>4851*1.34*1.09</f>
-        <v>7085.3706000000011</v>
+        <f>4851*1.34*1.08</f>
+        <v>7020.3672000000006</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1591,8 +1591,8 @@
         <v>27</v>
       </c>
       <c r="F15">
-        <f>374*19.94*1.09</f>
-        <v>8128.7404000000006</v>
+        <f>374*19.94*1.08</f>
+        <v>8054.1648000000014</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -1613,8 +1613,8 @@
         <v>12</v>
       </c>
       <c r="F16">
-        <f>7464*0.43*1.09</f>
-        <v>3498.3768000000005</v>
+        <f>7464*0.43*1.08</f>
+        <v>3466.2816000000003</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -1635,8 +1635,8 @@
         <v>12</v>
       </c>
       <c r="F17">
-        <f>7161*22.33*1.09</f>
-        <v>174296.59169999999</v>
+        <f>7161*22.33*1.08</f>
+        <v>172697.5404</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -1657,8 +1657,8 @@
         <v>12</v>
       </c>
       <c r="F18">
-        <f>1785*13.45*1.09</f>
-        <v>26168.9925</v>
+        <f>1785*13.45*1.08</f>
+        <v>25928.910000000003</v>
       </c>
       <c r="G18" s="1"/>
     </row>
@@ -1679,8 +1679,8 @@
         <v>12</v>
       </c>
       <c r="F19">
-        <f>43*26.07*1.09</f>
-        <v>1221.9009000000001</v>
+        <f>43*26.07*1.08</f>
+        <v>1210.6908000000001</v>
       </c>
       <c r="G19" s="1"/>
     </row>
@@ -1701,8 +1701,8 @@
         <v>12</v>
       </c>
       <c r="F20">
-        <f>2684*1.3*1.09</f>
-        <v>3803.2280000000005</v>
+        <f>2684*1.3*1.08</f>
+        <v>3768.3360000000007</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -1723,8 +1723,8 @@
         <v>12</v>
       </c>
       <c r="F21">
-        <f>1965*25.05*1.09</f>
-        <v>53653.342500000006</v>
+        <f>1965*25.05*1.08</f>
+        <v>53161.11</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -1745,8 +1745,8 @@
         <v>27</v>
       </c>
       <c r="F22">
-        <f>2477*2.32*1.09</f>
-        <v>6263.8375999999998</v>
+        <f>2477*2.32*1.08</f>
+        <v>6206.3711999999996</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -1789,8 +1789,8 @@
         <v>12</v>
       </c>
       <c r="F24">
-        <f>502*19.27*1.09</f>
-        <v>10544.158599999999</v>
+        <f>502*19.27*1.08</f>
+        <v>10447.423199999999</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -1811,8 +1811,8 @@
         <v>12</v>
       </c>
       <c r="F25">
-        <f>3636*26.98*1.09</f>
-        <v>106928.21520000001</v>
+        <f>3636*26.98*1.08</f>
+        <v>105947.2224</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -1833,8 +1833,8 @@
         <v>12</v>
       </c>
       <c r="F26">
-        <f>3372*14.19*1.09</f>
-        <v>52155.061200000004</v>
+        <f>3372*14.19*1.08</f>
+        <v>51676.574400000005</v>
       </c>
       <c r="G26" s="1"/>
     </row>
@@ -1877,8 +1877,8 @@
         <v>12</v>
       </c>
       <c r="F28">
-        <f>7537*20*1.09</f>
-        <v>164306.6</v>
+        <f>7537*20*1.08</f>
+        <v>162799.20000000001</v>
       </c>
       <c r="G28" s="1"/>
     </row>
@@ -1899,8 +1899,8 @@
         <v>12</v>
       </c>
       <c r="F29">
-        <f>7344*14.5*1.09</f>
-        <v>116071.92000000001</v>
+        <f>7344*14.5*1.08</f>
+        <v>115007.04000000001</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -1921,8 +1921,8 @@
         <v>44</v>
       </c>
       <c r="F30">
-        <f>5267*0.59*1.09</f>
-        <v>3387.2076999999999</v>
+        <f>5267*0.59*1.08</f>
+        <v>3356.1324</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -1943,8 +1943,8 @@
         <v>12</v>
       </c>
       <c r="F31">
-        <f>5002*8.95*1.09</f>
-        <v>48797.010999999999</v>
+        <f>5002*8.95*1.08</f>
+        <v>48349.331999999995</v>
       </c>
       <c r="G31" s="1"/>
     </row>
@@ -1965,8 +1965,8 @@
         <v>12</v>
       </c>
       <c r="F32">
-        <f>1623*27.25*1.09</f>
-        <v>48207.157500000001</v>
+        <f>1623*27.25*1.08</f>
+        <v>47764.890000000007</v>
       </c>
       <c r="G32" s="1"/>
     </row>
@@ -1987,8 +1987,8 @@
         <v>17</v>
       </c>
       <c r="F33">
-        <f>5951*13.55*0.094</f>
-        <v>7579.7887000000001</v>
+        <f>5951*13.55*0.093</f>
+        <v>7499.15265</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -2009,8 +2009,8 @@
         <v>12</v>
       </c>
       <c r="F34">
-        <f>5100*9.44*1.09</f>
-        <v>52476.960000000006</v>
+        <f>5100*9.44*1.08</f>
+        <v>51995.520000000004</v>
       </c>
       <c r="G34" s="1"/>
     </row>
@@ -2031,8 +2031,8 @@
         <v>27</v>
       </c>
       <c r="F35">
-        <f>5565*2.86*1.09</f>
-        <v>17348.331000000002</v>
+        <f>5565*2.86*1.08</f>
+        <v>17189.172000000002</v>
       </c>
       <c r="G35" s="1"/>
     </row>
@@ -2053,8 +2053,8 @@
         <v>12</v>
       </c>
       <c r="F36">
-        <f>6381*1.86*1.09</f>
-        <v>12936.839400000001</v>
+        <f>6381*1.86*1.08</f>
+        <v>12818.1528</v>
       </c>
       <c r="G36" s="1"/>
     </row>
@@ -2075,8 +2075,8 @@
         <v>12</v>
       </c>
       <c r="F37">
-        <f>8595*14.89*1.09</f>
-        <v>139497.70950000003</v>
+        <f>8595*14.89*1.08</f>
+        <v>138217.91400000002</v>
       </c>
       <c r="G37" s="1"/>
     </row>
@@ -2097,8 +2097,8 @@
         <v>44</v>
       </c>
       <c r="F38">
-        <f>1480*7.46*1.09</f>
-        <v>12034.472</v>
+        <f>1480*7.46*1.08</f>
+        <v>11924.064</v>
       </c>
       <c r="G38" s="1"/>
     </row>
@@ -2119,8 +2119,8 @@
         <v>12</v>
       </c>
       <c r="F39">
-        <f>455*23.04*1.09</f>
-        <v>11426.688</v>
+        <f>455*23.04*1.08</f>
+        <v>11321.856</v>
       </c>
       <c r="G39" s="1"/>
     </row>
@@ -2141,8 +2141,8 @@
         <v>12</v>
       </c>
       <c r="F40">
-        <f>3501*18.35*1.09</f>
-        <v>70025.251500000013</v>
+        <f>3501*18.35*1.08</f>
+        <v>69382.818000000014</v>
       </c>
       <c r="G40" s="1"/>
     </row>
@@ -2163,8 +2163,8 @@
         <v>12</v>
       </c>
       <c r="F41">
-        <f>3793*6.08*1.09</f>
-        <v>25136.9696</v>
+        <f>3793*6.08*1.08</f>
+        <v>24906.355200000002</v>
       </c>
       <c r="G41" s="1"/>
     </row>
@@ -2185,8 +2185,8 @@
         <v>27</v>
       </c>
       <c r="F42">
-        <f>3633*19.7*1.09</f>
-        <v>78011.409</v>
+        <f>3633*19.7*1.08</f>
+        <v>77295.707999999999</v>
       </c>
       <c r="G42" s="1"/>
     </row>
@@ -2207,8 +2207,8 @@
         <v>12</v>
       </c>
       <c r="F43">
-        <f>3677*25.83*1.09</f>
-        <v>103524.83189999999</v>
+        <f>3677*25.83*1.08</f>
+        <v>102575.0628</v>
       </c>
       <c r="G43" s="1"/>
     </row>
@@ -2229,8 +2229,8 @@
         <v>12</v>
       </c>
       <c r="F44">
-        <f>324*21.52*1.09</f>
-        <v>7600.0032000000001</v>
+        <f>324*21.52*1.08</f>
+        <v>7530.2784000000001</v>
       </c>
       <c r="G44" s="1"/>
     </row>
@@ -2251,8 +2251,8 @@
         <v>17</v>
       </c>
       <c r="F45">
-        <f>3998*19.47*0.094</f>
-        <v>7317.0596399999995</v>
+        <f>3998*19.47*0.093</f>
+        <v>7239.2185799999997</v>
       </c>
       <c r="G45" s="1"/>
     </row>
@@ -2273,8 +2273,8 @@
         <v>17</v>
       </c>
       <c r="F46">
-        <f>1996*20.09*0.094</f>
-        <v>3769.36616</v>
+        <f>1996*20.09*0.093</f>
+        <v>3729.2665200000001</v>
       </c>
       <c r="G46" s="1"/>
     </row>
@@ -2295,8 +2295,8 @@
         <v>17</v>
       </c>
       <c r="F47">
-        <f>5990*2.05*0.094</f>
-        <v>1154.2729999999999</v>
+        <f>5990*2.05*0.093</f>
+        <v>1141.9934999999998</v>
       </c>
       <c r="G47" s="1"/>
     </row>
@@ -2317,8 +2317,8 @@
         <v>12</v>
       </c>
       <c r="F48">
-        <f>7160*23.23*1.09</f>
-        <v>181296.21200000003</v>
+        <f>7160*23.23*1.08</f>
+        <v>179632.94400000002</v>
       </c>
       <c r="G48" s="1"/>
     </row>
@@ -2339,8 +2339,8 @@
         <v>12</v>
       </c>
       <c r="F49">
-        <f>6880*8.88*1.09</f>
-        <v>66592.896000000008</v>
+        <f>6880*8.88*1.08</f>
+        <v>65981.952000000019</v>
       </c>
       <c r="G49" s="1"/>
     </row>
@@ -2399,7 +2399,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>1.0900000000000001</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2415,7 +2415,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>9.4E-2</v>
+        <v>9.2999999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>